<commit_message>
refactor: fixing folders structure
</commit_message>
<xml_diff>
--- a/SysCall-BackEnd/Documentações/Dicionario de Dados - SysCall.xlsx
+++ b/SysCall-BackEnd/Documentações/Dicionario de Dados - SysCall.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapha\Desktop\SysCall\SysCall-BackEnd\Dicionario de Dados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rsilva\Desktop\Syscall\SysCall-BackEnd\Documentações\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F726D13-D500-4F75-B9CF-7E37BBE5FCD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11040"/>
+    <workbookView xWindow="-2040" yWindow="-13620" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -20,28 +21,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Raphael Silva</author>
   </authors>
   <commentList>
-    <comment ref="F13" authorId="0" shapeId="0">
+    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -65,12 +55,37 @@
         </r>
       </text>
     </comment>
+    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{8F0AEA5A-B0DD-40D3-B095-DDA9E8E9BA05}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t>Raphael Silva:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Chave única composta pelo saved_user e owner_user
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="64">
   <si>
     <t>auth.users</t>
   </si>
@@ -255,20 +270,20 @@
     <t>sys_call.call_history</t>
   </si>
   <si>
-    <t>CURRENT_TIME</t>
-  </si>
-  <si>
     <t>duration</t>
   </si>
   <si>
     <t>INTERVAL</t>
+  </si>
+  <si>
+    <t>CURRENT_TIMESTAMP</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -343,7 +358,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="30">
     <border>
       <left/>
       <right/>
@@ -707,11 +722,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -785,24 +813,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -822,29 +832,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1183,56 +1202,56 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:L49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I45" sqref="I45"/>
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.8984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.69921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="48.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="48.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.3984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" ht="14.4" thickBot="1"/>
-    <row r="4" spans="1:12" ht="14.4" thickBot="1">
-      <c r="B4" s="26" t="s">
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="28"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="39"/>
       <c r="J4" s="6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="14.4" thickBot="1">
-      <c r="B5" s="29"/>
-      <c r="C5" s="30"/>
-      <c r="D5" s="30"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="30"/>
-      <c r="H5" s="31"/>
-      <c r="J5" s="38" t="s">
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="40"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="42"/>
+      <c r="J5" s="32" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:12" ht="14.4" thickBot="1">
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
@@ -1254,11 +1273,11 @@
       <c r="H6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J6" s="34" t="s">
+      <c r="J6" s="28" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
         <v>24</v>
       </c>
@@ -1281,7 +1300,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="15">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B8" s="10" t="s">
         <v>2</v>
       </c>
@@ -1304,7 +1323,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="15">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="1" t="s">
         <v>3</v>
@@ -1328,7 +1347,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" s="10" t="s">
         <v>54</v>
       </c>
@@ -1351,7 +1370,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="15">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="s">
         <v>4</v>
       </c>
@@ -1374,7 +1393,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="15">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
         <v>53</v>
       </c>
@@ -1397,7 +1416,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="s">
         <v>5</v>
       </c>
@@ -1408,7 +1427,7 @@
         <v>22</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>14</v>
@@ -1420,11 +1439,11 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:12" ht="14.4" thickBot="1">
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="33" t="s">
         <v>23</v>
       </c>
       <c r="D14" s="14" t="s">
@@ -1443,14 +1462,14 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="1"/>
       <c r="H15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1460,7 +1479,7 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1471,7 +1490,7 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -1482,38 +1501,38 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="22" spans="1:12" ht="14.4" thickBot="1">
-      <c r="J22" s="35"/>
-    </row>
-    <row r="23" spans="1:12" ht="14.4" thickBot="1">
-      <c r="B23" s="26" t="s">
+    <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J22" s="29"/>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="32"/>
+      <c r="C23" s="38"/>
+      <c r="D23" s="38"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="39"/>
+      <c r="I23" s="26"/>
       <c r="J23" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="15.6" thickBot="1">
-      <c r="B24" s="29"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="31"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="36" t="s">
+    <row r="24" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="40"/>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="26"/>
+      <c r="J24" s="30" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:12" ht="14.4" thickBot="1">
+    <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
         <v>1</v>
       </c>
@@ -1535,12 +1554,12 @@
       <c r="H25" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I25" s="32"/>
-      <c r="J25" s="34" t="s">
+      <c r="I25" s="26"/>
+      <c r="J25" s="28" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B26" s="6" t="s">
         <v>24</v>
       </c>
@@ -1562,9 +1581,9 @@
       <c r="H26" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="J26" s="33"/>
-    </row>
-    <row r="27" spans="1:12">
+      <c r="J26" s="27"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B27" s="10" t="s">
         <v>25</v>
       </c>
@@ -1575,7 +1594,7 @@
         <v>13</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="F27" s="12" t="s">
         <v>46</v>
@@ -1587,7 +1606,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:12" ht="15">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
       <c r="B28" s="1" t="s">
         <v>26</v>
@@ -1611,7 +1630,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29" s="10" t="s">
         <v>55</v>
       </c>
@@ -1624,8 +1643,8 @@
       <c r="E29" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="12" t="s">
-        <v>46</v>
+      <c r="F29" s="43" t="s">
+        <v>14</v>
       </c>
       <c r="G29" s="12" t="s">
         <v>46</v>
@@ -1634,11 +1653,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="14.4" thickBot="1">
+    <row r="30" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="39" t="s">
+      <c r="C30" s="33" t="s">
         <v>12</v>
       </c>
       <c r="D30" s="12" t="s">
@@ -1647,9 +1666,7 @@
       <c r="E30" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="F30" s="14" t="s">
-        <v>46</v>
-      </c>
+      <c r="F30" s="44"/>
       <c r="G30" s="15" t="s">
         <v>46</v>
       </c>
@@ -1657,17 +1674,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:12">
-      <c r="B31" s="40"/>
-      <c r="C31" s="40"/>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
       <c r="H31" s="7"/>
     </row>
-    <row r="32" spans="1:12">
-      <c r="B32" s="40"/>
-      <c r="C32" s="40"/>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -1676,9 +1693,9 @@
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="2:12">
-      <c r="B33" s="40"/>
-      <c r="C33" s="40"/>
+    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -1689,9 +1706,9 @@
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
     </row>
-    <row r="34" spans="2:12">
-      <c r="B34" s="40"/>
-      <c r="C34" s="40"/>
+    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -1702,35 +1719,34 @@
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
     </row>
-    <row r="36" spans="2:12" ht="15"/>
-    <row r="37" spans="2:12" ht="14.4" thickBot="1"/>
-    <row r="38" spans="2:12" ht="14.4" thickBot="1">
-      <c r="B38" s="26" t="s">
+    <row r="37" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="38" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="37" t="s">
         <v>60</v>
       </c>
-      <c r="C38" s="27"/>
-      <c r="D38" s="27"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="28"/>
+      <c r="C38" s="38"/>
+      <c r="D38" s="38"/>
+      <c r="E38" s="38"/>
+      <c r="F38" s="38"/>
+      <c r="G38" s="38"/>
+      <c r="H38" s="39"/>
       <c r="J38" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="2:12" ht="14.4" thickBot="1">
-      <c r="B39" s="29"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="31"/>
-      <c r="J39" s="37" t="s">
+    <row r="39" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="40"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="41"/>
+      <c r="E39" s="41"/>
+      <c r="F39" s="41"/>
+      <c r="G39" s="41"/>
+      <c r="H39" s="42"/>
+      <c r="J39" s="31" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="2:12" ht="14.4" thickBot="1">
+    <row r="40" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="2" t="s">
         <v>1</v>
       </c>
@@ -1753,7 +1769,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="2:12">
+    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
         <v>24</v>
       </c>
@@ -1776,7 +1792,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="2:12">
+    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B42" s="10" t="s">
         <v>26</v>
       </c>
@@ -1799,7 +1815,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="43" spans="2:12">
+    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B43" s="16" t="s">
         <v>28</v>
       </c>
@@ -1816,36 +1832,36 @@
         <v>46</v>
       </c>
       <c r="G43" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="H43" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B44" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="H43" s="24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="44" spans="2:12">
-      <c r="B44" s="41" t="s">
+      <c r="C44" s="34" t="s">
         <v>62</v>
       </c>
-      <c r="C44" s="43" t="s">
-        <v>63</v>
-      </c>
-      <c r="D44" s="44" t="s">
+      <c r="D44" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="E44" s="46" t="s">
-        <v>46</v>
-      </c>
-      <c r="F44" s="45" t="s">
-        <v>46</v>
-      </c>
-      <c r="G44" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="H44" s="47" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="45" spans="2:12">
+      <c r="E44" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F44" s="36" t="s">
+        <v>46</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H44" s="24" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B45" s="10" t="s">
         <v>57</v>
       </c>
@@ -1868,11 +1884,11 @@
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="2:12" ht="14.4" thickBot="1">
+    <row r="46" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C46" s="39" t="s">
+      <c r="C46" s="33" t="s">
         <v>12</v>
       </c>
       <c r="D46" s="15" t="s">
@@ -1891,7 +1907,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="2:12">
+    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D47" s="1"/>
       <c r="E47" s="7"/>
       <c r="F47" s="1"/>
@@ -1900,7 +1916,7 @@
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
     </row>
-    <row r="48" spans="2:12">
+    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -1911,7 +1927,7 @@
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
     </row>
-    <row r="49" spans="4:12">
+    <row r="49" spans="4:12" x14ac:dyDescent="0.25">
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -1923,10 +1939,11 @@
       <c r="L49" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="B4:H5"/>
     <mergeCell ref="B23:H24"/>
     <mergeCell ref="B38:H39"/>
+    <mergeCell ref="F29:F30"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <legacyDrawing r:id="rId1"/>
@@ -1934,20 +1951,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="C2:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:4" ht="15.75" thickBot="1"/>
-    <row r="3" spans="3:4" ht="15.75" thickBot="1">
+    <row r="2" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="22" t="s">
         <v>43</v>
       </c>
@@ -1955,7 +1972,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="3:4" ht="15">
+    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C4" s="19" t="s">
         <v>30</v>
       </c>
@@ -1963,7 +1980,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="3:4" ht="15">
+    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C5" s="18" t="s">
         <v>33</v>
       </c>
@@ -1971,7 +1988,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="3:4" ht="15">
+    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C6" s="18" t="s">
         <v>31</v>
       </c>
@@ -1979,7 +1996,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="3:4" ht="15">
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C7" s="18" t="s">
         <v>38</v>
       </c>
@@ -1987,7 +2004,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="3:4" ht="15">
+    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C8" s="18" t="s">
         <v>34</v>
       </c>
@@ -2010,6 +2027,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BDF39B024F04A14486BA613BEA42AFF1" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="48c91588e4c96d3b87372e2739b705e1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="87289aac-3191-415d-94b6-004c2ae78a31" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0362d00d4c3829c3077b766beca3d16d" ns3:_="">
     <xsd:import namespace="87289aac-3191-415d-94b6-004c2ae78a31"/>
@@ -2153,12 +2176,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{318E7733-B127-4355-B93C-6EC54A543DCE}">
   <ds:schemaRefs>
@@ -2168,6 +2185,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12E806BA-4CE2-430B-BCC3-C1004ADA0620}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="87289aac-3191-415d-94b6-004c2ae78a31"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D2CE125-FEC1-4111-B9B7-3D153BF8148D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2183,20 +2216,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12E806BA-4CE2-430B-BCC3-C1004ADA0620}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87289aac-3191-415d-94b6-004c2ae78a31"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
feat: creating function to populate call_history table and fix doc issues
</commit_message>
<xml_diff>
--- a/SysCall-BackEnd/Documentações/Dicionario de Dados - SysCall.xlsx
+++ b/SysCall-BackEnd/Documentações/Dicionario de Dados - SysCall.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rsilva\Desktop\Syscall\SysCall-BackEnd\Documentações\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rapha\Desktop\SysCall\SysCall-BackEnd\Documentações\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F726D13-D500-4F75-B9CF-7E37BBE5FCD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2040" yWindow="-13620" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-2040" yWindow="-13620" windowWidth="24240" windowHeight="13020"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -26,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>Raphael Silva</author>
   </authors>
   <commentList>
-    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="F13" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -55,7 +54,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{8F0AEA5A-B0DD-40D3-B095-DDA9E8E9BA05}">
+    <comment ref="F29" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -156,9 +155,6 @@
     <t>NULL</t>
   </si>
   <si>
-    <t>DOMAIN_LOCATION</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
@@ -277,13 +273,16 @@
   </si>
   <si>
     <t>CURRENT_TIMESTAMP</t>
+  </si>
+  <si>
+    <t>CHAR(2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +330,14 @@
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -739,7 +746,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -865,6 +872,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1202,30 +1210,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:L49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="2" max="2" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.8984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.296875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="48.3984375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="25" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="48.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="48.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" ht="15.75" thickBot="1"/>
+    <row r="4" spans="1:12" ht="14.4" thickBot="1">
       <c r="B4" s="37" t="s">
         <v>0</v>
       </c>
@@ -1239,7 +1247,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="14.4" thickBot="1">
       <c r="B5" s="40"/>
       <c r="C5" s="41"/>
       <c r="D5" s="41"/>
@@ -1248,10 +1256,10 @@
       <c r="G5" s="41"/>
       <c r="H5" s="42"/>
       <c r="J5" s="32" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="14.4" thickBot="1">
       <c r="B6" s="2" t="s">
         <v>1</v>
       </c>
@@ -1262,7 +1270,7 @@
         <v>8</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>9</v>
@@ -1274,12 +1282,12 @@
         <v>11</v>
       </c>
       <c r="J6" s="28" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15">
       <c r="B7" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>12</v>
@@ -1288,19 +1296,19 @@
         <v>13</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H7" s="23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="15">
       <c r="B8" s="10" t="s">
         <v>2</v>
       </c>
@@ -1311,19 +1319,19 @@
         <v>22</v>
       </c>
       <c r="E8" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H8" s="24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15">
       <c r="A9" s="5"/>
       <c r="B9" s="1" t="s">
         <v>3</v>
@@ -1335,21 +1343,21 @@
         <v>22</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G9" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H9" s="24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="15">
       <c r="B10" s="10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" s="11" t="s">
         <v>18</v>
@@ -1358,19 +1366,19 @@
         <v>22</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H10" s="24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15">
       <c r="B11" s="10" t="s">
         <v>4</v>
       </c>
@@ -1381,21 +1389,21 @@
         <v>13</v>
       </c>
       <c r="E11" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G11" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15">
       <c r="B12" s="10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C12" s="11" t="s">
         <v>20</v>
@@ -1404,19 +1412,19 @@
         <v>13</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H12" s="24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15">
       <c r="B13" s="10" t="s">
         <v>5</v>
       </c>
@@ -1427,49 +1435,49 @@
         <v>22</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F13" s="12" t="s">
         <v>14</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" thickBot="1">
       <c r="B14" s="13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>23</v>
+        <v>63</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>22</v>
       </c>
       <c r="E14" s="14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G14" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H14" s="25" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="15">
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="1"/>
       <c r="H15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="15">
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -1479,7 +1487,7 @@
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" ht="15">
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
@@ -1490,7 +1498,7 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" ht="15">
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -1501,12 +1509,15 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12">
+      <c r="E21" s="45"/>
+    </row>
+    <row r="22" spans="1:12" ht="15.75" thickBot="1">
       <c r="J22" s="29"/>
     </row>
-    <row r="23" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="14.4" thickBot="1">
       <c r="B23" s="37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C23" s="38"/>
       <c r="D23" s="38"/>
@@ -1519,7 +1530,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="15.6" thickBot="1">
       <c r="B24" s="40"/>
       <c r="C24" s="41"/>
       <c r="D24" s="41"/>
@@ -1529,10 +1540,10 @@
       <c r="H24" s="42"/>
       <c r="I24" s="26"/>
       <c r="J24" s="30" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="14.4" thickBot="1">
       <c r="B25" s="2" t="s">
         <v>1</v>
       </c>
@@ -1543,7 +1554,7 @@
         <v>8</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F25" s="2" t="s">
         <v>9</v>
@@ -1556,12 +1567,12 @@
       </c>
       <c r="I25" s="26"/>
       <c r="J25" s="28" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15">
       <c r="B26" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" s="8" t="s">
         <v>12</v>
@@ -1570,22 +1581,22 @@
         <v>13</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F26" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G26" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H26" s="23" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J26" s="27"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="15">
       <c r="B27" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" s="11" t="s">
         <v>19</v>
@@ -1594,45 +1605,45 @@
         <v>13</v>
       </c>
       <c r="E27" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G27" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H27" s="24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15">
       <c r="A28" s="5"/>
       <c r="B28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>27</v>
       </c>
       <c r="D28" s="12" t="s">
         <v>13</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H28" s="24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
       <c r="B29" s="10" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C29" s="11" t="s">
         <v>12</v>
@@ -1641,21 +1652,21 @@
         <v>13</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F29" s="43" t="s">
         <v>14</v>
       </c>
       <c r="G29" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H29" s="24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" ht="14.4" thickBot="1">
       <c r="B30" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C30" s="33" t="s">
         <v>12</v>
@@ -1664,17 +1675,17 @@
         <v>13</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F30" s="44"/>
       <c r="G30" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H30" s="25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="15">
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="7"/>
@@ -1682,7 +1693,7 @@
       <c r="F31" s="7"/>
       <c r="H31" s="7"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="15">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
@@ -1693,7 +1704,7 @@
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
     </row>
-    <row r="33" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:12" ht="15">
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
@@ -1706,7 +1717,7 @@
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
     </row>
-    <row r="34" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:12" ht="15">
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
@@ -1719,10 +1730,10 @@
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
     </row>
-    <row r="37" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="38" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:12" ht="15.75" thickBot="1"/>
+    <row r="38" spans="2:12" ht="14.4" thickBot="1">
       <c r="B38" s="37" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C38" s="38"/>
       <c r="D38" s="38"/>
@@ -1734,7 +1745,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:12" ht="14.4" thickBot="1">
       <c r="B39" s="40"/>
       <c r="C39" s="41"/>
       <c r="D39" s="41"/>
@@ -1743,10 +1754,10 @@
       <c r="G39" s="41"/>
       <c r="H39" s="42"/>
       <c r="J39" s="31" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="40" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12" ht="14.4" thickBot="1">
       <c r="B40" s="2" t="s">
         <v>1</v>
       </c>
@@ -1757,7 +1768,7 @@
         <v>8</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>9</v>
@@ -1769,9 +1780,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="41" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:12">
       <c r="B41" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C41" s="8" t="s">
         <v>12</v>
@@ -1780,90 +1791,90 @@
         <v>13</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F41" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G41" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H41" s="23" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="42" spans="2:12" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12">
       <c r="B42" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C42" s="11" t="s">
         <v>26</v>
-      </c>
-      <c r="C42" s="11" t="s">
-        <v>27</v>
       </c>
       <c r="D42" s="12" t="s">
         <v>13</v>
       </c>
       <c r="E42" s="12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F42" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G42" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H42" s="24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="43" spans="2:12" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12">
       <c r="B43" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="C43" s="11" t="s">
         <v>28</v>
-      </c>
-      <c r="C43" s="11" t="s">
-        <v>29</v>
       </c>
       <c r="D43" s="12" t="s">
         <v>13</v>
       </c>
       <c r="E43" s="12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F43" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G43" s="12" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H43" s="24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="44" spans="2:12" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12">
       <c r="B44" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C44" s="34" t="s">
         <v>61</v>
-      </c>
-      <c r="C44" s="34" t="s">
-        <v>62</v>
       </c>
       <c r="D44" s="35" t="s">
         <v>13</v>
       </c>
       <c r="E44" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F44" s="36" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H44" s="24" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12">
       <c r="B45" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C45" s="11" t="s">
         <v>12</v>
@@ -1872,21 +1883,21 @@
         <v>13</v>
       </c>
       <c r="E45" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F45" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G45" s="12" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H45" s="24" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="46" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:12" ht="14.4" thickBot="1">
       <c r="B46" s="13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C46" s="33" t="s">
         <v>12</v>
@@ -1895,19 +1906,19 @@
         <v>13</v>
       </c>
       <c r="E46" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G46" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H46" s="25" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="47" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:12">
       <c r="D47" s="1"/>
       <c r="E47" s="7"/>
       <c r="F47" s="1"/>
@@ -1916,7 +1927,7 @@
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
     </row>
-    <row r="48" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:12">
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -1927,7 +1938,7 @@
       <c r="K48" s="1"/>
       <c r="L48" s="1"/>
     </row>
-    <row r="49" spans="4:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:12">
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -1946,70 +1957,71 @@
     <mergeCell ref="F29:F30"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C2:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="3:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:4" ht="15.75" thickBot="1"/>
+    <row r="3" spans="3:4" ht="15.75" thickBot="1">
       <c r="C3" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="21" t="s">
+    </row>
+    <row r="4" spans="3:4" ht="15">
+      <c r="C4" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" ht="15">
+      <c r="C5" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" ht="15">
+      <c r="C6" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4" ht="15">
+      <c r="C7" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="17" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C4" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C5" s="18" t="s">
+    <row r="8" spans="3:4" ht="15">
+      <c r="C8" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="6" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C6" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="17" t="s">
+      <c r="D8" s="17" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C7" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C8" s="18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -2018,21 +2030,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BDF39B024F04A14486BA613BEA42AFF1" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="48c91588e4c96d3b87372e2739b705e1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="87289aac-3191-415d-94b6-004c2ae78a31" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0362d00d4c3829c3077b766beca3d16d" ns3:_="">
     <xsd:import namespace="87289aac-3191-415d-94b6-004c2ae78a31"/>
@@ -2176,31 +2173,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{318E7733-B127-4355-B93C-6EC54A543DCE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12E806BA-4CE2-430B-BCC3-C1004ADA0620}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="87289aac-3191-415d-94b6-004c2ae78a31"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D2CE125-FEC1-4111-B9B7-3D153BF8148D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2216,4 +2204,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{12E806BA-4CE2-430B-BCC3-C1004ADA0620}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="87289aac-3191-415d-94b6-004c2ae78a31"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{318E7733-B127-4355-B93C-6EC54A543DCE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>